<commit_message>
aprendendo algumas funções a mais
</commit_message>
<xml_diff>
--- a/nomes.xlsx
+++ b/nomes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -43,15 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="A2:B4"/>
@@ -432,8 +432,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="21.140625"/>
-    <col customWidth="1" max="2" min="2" width="26.28515625"/>
+    <col width="21.140625" customWidth="1" min="1" max="1"/>
+    <col width="26.28515625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,7 +488,14 @@
         <v>99</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ALUNOS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.787401575" footer="0.31496062" header="0.31496062" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>